<commit_message>
4/12/18 continued work on slided and calculations of test cases
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/FromOFFT_testcases_count.xlsx
+++ b/CurrentWork_Delta/FromOFFT_testcases_count.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="408" windowWidth="15096" windowHeight="4656"/>
+    <workbookView xWindow="0" yWindow="1005" windowWidth="5835" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>CA</t>
   </si>
@@ -135,6 +135,39 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>ape2e</t>
+  </si>
+  <si>
+    <t>bkp</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>deps</t>
+  </si>
+  <si>
+    <t>dpe2e</t>
+  </si>
+  <si>
+    <t>e2eAP</t>
+  </si>
+  <si>
+    <t>facs</t>
+  </si>
+  <si>
+    <t>pays</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>pers</t>
+  </si>
+  <si>
+    <t>shop</t>
   </si>
 </sst>
 </file>
@@ -479,18 +512,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -528,7 +561,7 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -612,7 +645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -698,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -784,7 +817,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -870,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -956,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -970,7 +1003,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1083,7 +1116,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1106,6 +1139,266 @@
       <c r="AB10">
         <f>SUM(V8:AB8)</f>
         <v>3234</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>72</v>
+      </c>
+      <c r="H19">
+        <f>C19</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>136</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G29" si="1">C20</f>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <f>C21</f>
+        <v>63</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H20:H29" si="2">C21</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <f>C22</f>
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F20:F29" si="3">C22</f>
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>108</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24">
+        <v>110</v>
+      </c>
+      <c r="E24">
+        <f>C24</f>
+        <v>110</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>110</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ref="E25:E28" si="4">C25</f>
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28">
+        <v>122</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>122</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29">
+        <v>41</v>
+      </c>
+      <c r="E29">
+        <f>C29</f>
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" ref="C31:D31" si="5">SUM(C19:C29)</f>
+        <v>735</v>
+      </c>
+      <c r="E31">
+        <f>SUM(E19:E29)</f>
+        <v>411</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ref="F31:H31" si="6">SUM(F19:F29)</f>
+        <v>348</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="6"/>
+        <v>643</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="6"/>
+        <v>471</v>
+      </c>
+      <c r="J31">
+        <f>SUM(E31:H31)</f>
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>348</v>
+      </c>
+      <c r="H32">
+        <v>471</v>
+      </c>
+      <c r="J32">
+        <f>SUM(E32:H32)</f>
+        <v>819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4/12/18 mods to file
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/FromOFFT_testcases_count.xlsx
+++ b/CurrentWork_Delta/FromOFFT_testcases_count.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1005" windowWidth="5835" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="1416" windowWidth="5832" windowHeight="4656"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -514,16 +514,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="4" t="s">
         <v>5</v>
@@ -561,7 +561,7 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -645,7 +645,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -817,7 +817,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -989,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1003,7 +1003,7 @@
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E17" t="s">
         <v>33</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1167,19 +1167,27 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="C20">
         <v>136</v>
       </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
       <c r="G20">
-        <f t="shared" ref="G20:G29" si="1">C20</f>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1190,16 +1198,20 @@
         <f>C21</f>
         <v>63</v>
       </c>
+      <c r="F21">
+        <f>C21</f>
+        <v>63</v>
+      </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G20:G29" si="1">C21</f>
         <v>63</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H20:H29" si="2">C21</f>
+        <f t="shared" ref="H21:H29" si="2">C21</f>
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>38</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F20:F29" si="3">C22</f>
+        <f t="shared" ref="F22:F29" si="3">C22</f>
         <v>38</v>
       </c>
       <c r="G22">
@@ -1223,7 +1235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1247,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1299,11 +1311,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>45</v>
       </c>
       <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <f>C27</f>
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <f>C27</f>
         <v>8</v>
       </c>
       <c r="G27">
@@ -1315,7 +1335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1339,7 +1359,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1347,49 +1367,45 @@
         <v>41</v>
       </c>
       <c r="E29">
-        <f>C29</f>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <f t="shared" si="3"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C31">
-        <f t="shared" ref="C31:D31" si="5">SUM(C19:C29)</f>
+        <f t="shared" ref="C31" si="5">SUM(C19:C29)</f>
         <v>735</v>
       </c>
       <c r="E31">
         <f>SUM(E19:E29)</f>
-        <v>411</v>
+        <v>378</v>
       </c>
       <c r="F31">
         <f t="shared" ref="F31:H31" si="6">SUM(F19:F29)</f>
-        <v>348</v>
+        <v>378</v>
       </c>
       <c r="G31">
         <f t="shared" si="6"/>
-        <v>643</v>
+        <v>466</v>
       </c>
       <c r="H31">
         <f t="shared" si="6"/>
-        <v>471</v>
+        <v>430</v>
       </c>
       <c r="J31">
         <f>SUM(E31:H31)</f>
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F32">
         <v>348</v>
       </c>

</xml_diff>